<commit_message>
114 numaranın temmuz hakedişi eklendi
</commit_message>
<xml_diff>
--- a/Ofis Dosyalari/HAKEDISLER/2025/AĞUSTOS 2025/2025 AĞUSTOS AYI - AGREGA.xlsx
+++ b/Ofis Dosyalari/HAKEDISLER/2025/AĞUSTOS 2025/2025 AĞUSTOS AYI - AGREGA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samil\OneDrive\Desktop\OfisDosyalariYedegi\Ofis Dosyalari\HAKEDISLER\2025\AĞUSTOS 2025\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F6AE8CD-E6B6-45B4-896F-C86BA55F213A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F310D3E-CE49-4B8D-92A6-FC122C5880B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -985,17 +985,17 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1284,8 +1284,8 @@
   <dimension ref="A1:M70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K36" sqref="K36"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5546875" defaultRowHeight="14.4"/>
@@ -1304,20 +1304,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15" thickBot="1">
-      <c r="A1" s="78" t="s">
+      <c r="A1" s="81" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="78"/>
-      <c r="C1" s="78"/>
-      <c r="D1" s="78"/>
-      <c r="E1" s="78"/>
-      <c r="F1" s="78"/>
-      <c r="G1" s="78"/>
-      <c r="H1" s="78"/>
-      <c r="I1" s="78"/>
-      <c r="J1" s="78"/>
-      <c r="K1" s="78"/>
-      <c r="L1" s="78"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="81"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="81"/>
+      <c r="J1" s="81"/>
+      <c r="K1" s="81"/>
+      <c r="L1" s="81"/>
     </row>
     <row r="2" spans="1:13" ht="43.8" thickBot="1">
       <c r="A2" s="1" t="s">
@@ -1759,13 +1759,13 @@
       <c r="L14" s="15"/>
     </row>
     <row r="15" spans="1:13" ht="16.5" customHeight="1">
-      <c r="A15" s="79">
+      <c r="A15" s="78">
         <v>13</v>
       </c>
-      <c r="B15" s="80">
+      <c r="B15" s="79">
         <v>114</v>
       </c>
-      <c r="C15" s="81" t="s">
+      <c r="C15" s="80" t="s">
         <v>30</v>
       </c>
       <c r="D15" s="47">
@@ -1778,7 +1778,9 @@
         <f t="shared" si="0"/>
         <v>113570</v>
       </c>
-      <c r="G15" s="49"/>
+      <c r="G15" s="49">
+        <v>118090</v>
+      </c>
       <c r="H15" s="49">
         <v>67760</v>
       </c>
@@ -1790,7 +1792,7 @@
       </c>
       <c r="K15" s="51">
         <f t="shared" si="1"/>
-        <v>155330</v>
+        <v>273420</v>
       </c>
       <c r="L15" s="52"/>
       <c r="M15" s="53" t="s">
@@ -3627,7 +3629,7 @@
     <row r="70" spans="1:12" ht="15" thickBot="1">
       <c r="K70" s="40">
         <f>SUM(K3:K69)</f>
-        <v>10224220</v>
+        <v>10342310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>